<commit_message>
Módulo 14 - Tabela de contas de entradas
</commit_message>
<xml_diff>
--- a/Projeto Final/base-de-dados-1.xlsx
+++ b/Projeto Final/base-de-dados-1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
   <si>
     <t>Vendas de mercadorias</t>
   </si>
@@ -218,6 +218,24 @@
   <si>
     <t>Nível 2 - fetalhe</t>
   </si>
+  <si>
+    <t>Plano de contas de entrada nível 1</t>
+  </si>
+  <si>
+    <t>Nível 1</t>
+  </si>
+  <si>
+    <t>Financiamento de longo prazo</t>
+  </si>
+  <si>
+    <t>Receitas Financeiras</t>
+  </si>
+  <si>
+    <t>Vendas de mercadoria</t>
+  </si>
+  <si>
+    <t>Doações</t>
+  </si>
 </sst>
 </file>
 
@@ -226,7 +244,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,6 +264,22 @@
       <b/>
       <sz val="20"/>
       <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -277,7 +311,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -285,11 +319,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -303,11 +352,19 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -4971,6 +5028,16 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B4:B10"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nível 1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5262,7 +5329,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5290,7 +5359,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="2:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -6286,7 +6355,8 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6330,14 +6400,58 @@
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6348,6 +6462,9 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Módulo 14 - Configuração inicial das tabelas
</commit_message>
<xml_diff>
--- a/Projeto Final/base-de-dados-1.xlsx
+++ b/Projeto Final/base-de-dados-1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="3" r:id="rId1"/>
@@ -26,12 +26,16 @@
     <sheet name="Entradas" sheetId="1" r:id="rId17"/>
     <sheet name="Saídas" sheetId="2" r:id="rId18"/>
   </sheets>
+  <definedNames>
+    <definedName name="PcEntradasN1">TbPCEntradasN1[Nível 1]</definedName>
+    <definedName name="TBPCSaidasN1">Tabela3[Nível 1]</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="82">
   <si>
     <t>Vendas de mercadorias</t>
   </si>
@@ -231,10 +235,52 @@
     <t>Receitas Financeiras</t>
   </si>
   <si>
-    <t>Vendas de mercadoria</t>
-  </si>
-  <si>
     <t>Doações</t>
+  </si>
+  <si>
+    <t>Plano de contas de entrada - nível 2</t>
+  </si>
+  <si>
+    <t>Nível 2</t>
+  </si>
+  <si>
+    <t>Venda de mercadorias</t>
+  </si>
+  <si>
+    <t>Empréstimo de capital de giro</t>
+  </si>
+  <si>
+    <t>Juros sobre aplicações</t>
+  </si>
+  <si>
+    <t>Mobiliário próprio</t>
+  </si>
+  <si>
+    <t>Plano de contas de saída - nível 1</t>
+  </si>
+  <si>
+    <t>Despesas financeiras</t>
+  </si>
+  <si>
+    <t>Impostos de renda</t>
+  </si>
+  <si>
+    <t>Impostos sobre as vendas</t>
+  </si>
+  <si>
+    <t>Plano de contas de saídas - nível 2</t>
+  </si>
+  <si>
+    <t>Comunicação - Internet e telefonia</t>
+  </si>
+  <si>
+    <t>Juros sobre empréstimos</t>
+  </si>
+  <si>
+    <t>IR sobre o lucro presumido</t>
+  </si>
+  <si>
+    <t>Vestuário</t>
   </si>
 </sst>
 </file>
@@ -311,7 +357,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -321,16 +367,57 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="3" tint="-0.499984740745262"/>
+        <color theme="4" tint="-0.24994659260841701"/>
       </left>
       <right style="thin">
-        <color theme="3" tint="-0.499984740745262"/>
+        <color theme="4" tint="-0.24994659260841701"/>
       </right>
       <top style="thin">
-        <color theme="3" tint="-0.499984740745262"/>
+        <color theme="4" tint="-0.24994659260841701"/>
       </top>
       <bottom style="thin">
-        <color theme="3" tint="-0.499984740745262"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39994506668294322"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39994506668294322"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39994506668294322"/>
       </bottom>
       <diagonal/>
     </border>
@@ -338,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -352,8 +439,23 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5036,7 +5138,39 @@
   <tableColumns count="1">
     <tableColumn id="1" name="Nível 1"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C12" totalsRowShown="0">
+  <autoFilter ref="B4:C12"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nível 1"/>
+    <tableColumn id="2" name="Nível 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="B4:B10" totalsRowShown="0">
+  <autoFilter ref="B4:B10"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nível 1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="B4:C15" totalsRowShown="0">
+  <autoFilter ref="B4:C15"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nível 1"/>
+    <tableColumn id="2" name="Nível 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -5329,9 +5463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
-    </sheetView>
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5359,22 +5491,22 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-    </row>
-    <row r="3" spans="2:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+    </row>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>26</v>
       </c>
@@ -6354,9 +6486,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6401,7 +6533,7 @@
       <c r="N2" s="6"/>
     </row>
     <row r="3" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C3" s="6"/>
@@ -6418,7 +6550,7 @@
       <c r="N3" s="6"/>
     </row>
     <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>63</v>
       </c>
     </row>
@@ -6444,12 +6576,12 @@
     </row>
     <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6472,13 +6604,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="2" max="3" width="40.7109375" customWidth="1"/>
+    <col min="4" max="14" width="9.28515625" customWidth="1"/>
     <col min="15" max="15" width="9.140625" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
@@ -6515,24 +6650,114 @@
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B12">
+      <formula1>PcEntradasN1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -6541,7 +6766,8 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6585,14 +6811,58 @@
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+    </row>
     <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6603,22 +6873,26 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="2" max="3" width="40.7109375" customWidth="1"/>
+    <col min="4" max="14" width="9.28515625" customWidth="1"/>
     <col min="15" max="15" width="9.140625" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
@@ -6655,24 +6929,136 @@
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B15">
+      <formula1>TBPCSaidasN1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Módulo 14 - Registros de entradas
</commit_message>
<xml_diff>
--- a/Projeto Final/base-de-dados-1.xlsx
+++ b/Projeto Final/base-de-dados-1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="82">
   <si>
     <t>Vendas de mercadorias</t>
   </si>
@@ -287,7 +287,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
@@ -331,7 +332,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,6 +354,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -444,23 +451,88 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -4539,8 +4611,8 @@
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>66674</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>476250</xdr:rowOff>
     </xdr:to>
@@ -4552,7 +4624,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="295273" y="28575"/>
-          <a:ext cx="2705101" cy="447675"/>
+          <a:ext cx="2133602" cy="447675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5133,7 +5205,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="B4:B10"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Nível 1"/>
@@ -5171,6 +5243,22 @@
     <tableColumn id="2" name="Nível 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TbRegistroEntradas" displayName="TbRegistroEntradas" ref="B5:H9" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="B5:H9"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="8"/>
+    <tableColumn id="2" name="Data da Competência" dataDxfId="7"/>
+    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="6"/>
+    <tableColumn id="4" name="Conta Nível 1" dataDxfId="5"/>
+    <tableColumn id="5" name="Conta Nível 2" dataDxfId="4"/>
+    <tableColumn id="6" name="Histórico" dataDxfId="3"/>
+    <tableColumn id="7" name="Valor" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -5463,7 +5551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5492,19 +5580,19 @@
       </c>
     </row>
     <row r="2" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
     </row>
     <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -6047,7 +6135,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection sqref="A1:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6604,9 +6692,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6651,10 +6739,10 @@
       <c r="N2" s="6"/>
     </row>
     <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="13"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -6812,7 +6900,7 @@
       <c r="N2" s="6"/>
     </row>
     <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>73</v>
       </c>
       <c r="C3" s="6"/>
@@ -6883,7 +6971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
@@ -7066,37 +7154,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="6" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="45.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="9" max="14" width="7.7109375" customWidth="1"/>
     <col min="15" max="15" width="9.140625" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -7104,31 +7192,150 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-    </row>
-    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="3" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:8" s="22" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="18">
+        <v>43146</v>
+      </c>
+      <c r="C6" s="18">
+        <v>43146</v>
+      </c>
+      <c r="D6" s="18">
+        <v>43146</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="21">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="18">
+        <v>43530</v>
+      </c>
+      <c r="C7" s="18">
+        <v>43466</v>
+      </c>
+      <c r="D7" s="18">
+        <v>43496</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="21">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="18">
+        <v>43467</v>
+      </c>
+      <c r="C8" s="18">
+        <v>43467</v>
+      </c>
+      <c r="D8" s="18">
+        <v>43467</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="21">
+        <v>2689</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="18">
+        <v>43535</v>
+      </c>
+      <c r="C9" s="18">
+        <v>43467</v>
+      </c>
+      <c r="D9" s="18">
+        <v>43497</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="21">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+    </row>
+    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E9">
+      <formula1>PcEntradasN1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Módulo 14 - Registros com a função desloc
</commit_message>
<xml_diff>
--- a/Projeto Final/base-de-dados-1.xlsx
+++ b/Projeto Final/base-de-dados-1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="3" r:id="rId1"/>
@@ -28,14 +28,18 @@
   </sheets>
   <definedNames>
     <definedName name="PcEntradasN1">TbPCEntradasN1[Nível 1]</definedName>
+    <definedName name="PCEntradasN2_Nivel_1">TbPCEntradasN2[Nível 1]</definedName>
+    <definedName name="PCEntradasN2_Nivel2">TbPCEntradasN2[Nível 2]</definedName>
+    <definedName name="PcEntradasN2N1">TbPCEntradasN2[Nível 1]</definedName>
+    <definedName name="pcEntradasN2N2">TbPCEntradasN2[Nível 2]</definedName>
     <definedName name="TBPCSaidasN1">Tabela3[Nível 1]</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="83">
   <si>
     <t>Vendas de mercadorias</t>
   </si>
@@ -281,6 +285,9 @@
   </si>
   <si>
     <t>Vestuário</t>
+  </si>
+  <si>
+    <t>Geral</t>
   </si>
 </sst>
 </file>
@@ -455,14 +462,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -487,24 +486,19 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -532,6 +526,19 @@
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -5215,8 +5222,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C12" totalsRowShown="0">
-  <autoFilter ref="B4:C12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C13" totalsRowShown="0">
+  <autoFilter ref="B4:C13"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Nível 1"/>
     <tableColumn id="2" name="Nível 2"/>
@@ -5247,16 +5254,16 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TbRegistroEntradas" displayName="TbRegistroEntradas" ref="B5:H9" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TbRegistroEntradas" displayName="TbRegistroEntradas" ref="B5:H9" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="B5:H9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="8"/>
-    <tableColumn id="2" name="Data da Competência" dataDxfId="7"/>
-    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="6"/>
-    <tableColumn id="4" name="Conta Nível 1" dataDxfId="5"/>
-    <tableColumn id="5" name="Conta Nível 2" dataDxfId="4"/>
-    <tableColumn id="6" name="Histórico" dataDxfId="3"/>
-    <tableColumn id="7" name="Valor" dataDxfId="2"/>
+    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="6"/>
+    <tableColumn id="2" name="Data da Competência" dataDxfId="5"/>
+    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="4"/>
+    <tableColumn id="4" name="Conta Nível 1" dataDxfId="3"/>
+    <tableColumn id="5" name="Conta Nível 2" dataDxfId="2"/>
+    <tableColumn id="6" name="Histórico" dataDxfId="1"/>
+    <tableColumn id="7" name="Valor" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5551,7 +5558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A4" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6692,9 +6699,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6739,10 +6746,10 @@
       <c r="N2" s="6"/>
     </row>
     <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="23"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -6765,10 +6772,16 @@
     </row>
     <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
         <v>70</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -6827,7 +6840,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" t="s">
+        <v>82</v>
+      </c>
+    </row>
     <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6836,9 +6856,15 @@
   <mergeCells count="1">
     <mergeCell ref="B3:C3"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B12">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B13">
       <formula1>PcEntradasN1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5">
+      <formula1>PcEntradasN2N1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5">
+      <formula1>pcEntradasN2N2</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -6855,7 +6881,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6973,7 +6999,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7018,10 +7044,10 @@
       <c r="N2" s="6"/>
     </row>
     <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="17"/>
+      <c r="C3" s="25"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -7154,7 +7180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
@@ -7195,128 +7221,128 @@
     </row>
     <row r="3" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:8" s="22" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
+    <row r="5" spans="2:8" s="18" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="21" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="18">
+      <c r="B6" s="14">
         <v>43146</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="14">
         <v>43146</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="14">
         <v>43146</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="17">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="14">
+        <v>43530</v>
+      </c>
+      <c r="C7" s="14">
+        <v>43466</v>
+      </c>
+      <c r="D7" s="14">
+        <v>43496</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="17">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="14">
+        <v>43467</v>
+      </c>
+      <c r="C8" s="14">
+        <v>43467</v>
+      </c>
+      <c r="D8" s="14">
+        <v>43467</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="17">
+        <v>2689</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="14">
+        <v>43535</v>
+      </c>
+      <c r="C9" s="14">
+        <v>43467</v>
+      </c>
+      <c r="D9" s="14">
+        <v>43497</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="H6" s="21">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="18">
-        <v>43530</v>
-      </c>
-      <c r="C7" s="18">
-        <v>43466</v>
-      </c>
-      <c r="D7" s="18">
-        <v>43496</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="21">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="18">
-        <v>43467</v>
-      </c>
-      <c r="C8" s="18">
-        <v>43467</v>
-      </c>
-      <c r="D8" s="18">
-        <v>43467</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="21">
-        <v>2689</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="18">
-        <v>43535</v>
-      </c>
-      <c r="C9" s="18">
-        <v>43467</v>
-      </c>
-      <c r="D9" s="18">
-        <v>43497</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="17">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7326,9 +7352,18 @@
     <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E9">
       <formula1>PcEntradasN1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6">
+      <formula1>OFFSET(pcEntradasN2N2,MATCH(E6,PcEntradasN2N1,0)-1,0,COUNTIF(PcEntradasN2N1,E6))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11">
+      <formula1>OFFSET(pcEntradasN2N2,MATCH(E6,PcEntradasN2N1,0)-1,0,COUNTIF(PcEntradasN2N1,E6))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:F9">
+      <formula1>OFFSET(pcEntradasN2N2,MATCH(E6,PcEntradasN2N1,0)-1,0,COUNTIF(PcEntradasN2N1,E6))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Módulo 14 - Registros de saídas
</commit_message>
<xml_diff>
--- a/Projeto Final/base-de-dados-1.xlsx
+++ b/Projeto Final/base-de-dados-1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="3" r:id="rId1"/>
@@ -32,14 +32,15 @@
     <definedName name="PCEntradasN2_Nivel2">TbPCEntradasN2[Nível 2]</definedName>
     <definedName name="PcEntradasN2N1">TbPCEntradasN2[Nível 1]</definedName>
     <definedName name="pcEntradasN2N2">TbPCEntradasN2[Nível 2]</definedName>
-    <definedName name="TBPCSaidasN1">Tabela3[Nível 1]</definedName>
+    <definedName name="SaidasNivel1">TBSaidasNivel1[Nível 1]</definedName>
+    <definedName name="TBPCSaidasN1">TBSaidasNivel1[Nível 1]</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="83">
   <si>
     <t>Vendas de mercadorias</t>
   </si>
@@ -371,7 +372,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -435,11 +436,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -494,11 +508,106 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="21">
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -5212,7 +5321,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="20">
   <autoFilter ref="B4:B10"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Nível 1"/>
@@ -5233,7 +5342,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="B4:B10" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TBSaidasNivel1" displayName="TBSaidasNivel1" ref="B4:B10" totalsRowShown="0">
   <autoFilter ref="B4:B10"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Nível 1"/>
@@ -5254,14 +5363,30 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TbRegistroEntradas" displayName="TbRegistroEntradas" ref="B5:H9" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TbRegistroEntradas" displayName="TbRegistroEntradas" ref="B5:H9" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="B5:H9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="6"/>
-    <tableColumn id="2" name="Data da Competência" dataDxfId="5"/>
-    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="4"/>
-    <tableColumn id="4" name="Conta Nível 1" dataDxfId="3"/>
-    <tableColumn id="5" name="Conta Nível 2" dataDxfId="2"/>
+    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="17"/>
+    <tableColumn id="2" name="Data da Competência" dataDxfId="16"/>
+    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="15"/>
+    <tableColumn id="4" name="Conta Nível 1" dataDxfId="14"/>
+    <tableColumn id="5" name="Conta Nível 2" dataDxfId="13"/>
+    <tableColumn id="6" name="Histórico" dataDxfId="12"/>
+    <tableColumn id="7" name="Valor" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="TbRegistrosSaida" displayName="TbRegistrosSaida" ref="B5:H9" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3" headerRowBorderDxfId="9" tableBorderDxfId="10">
+  <autoFilter ref="B5:H9"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="8"/>
+    <tableColumn id="2" name="Data da Competência" dataDxfId="7"/>
+    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="6"/>
+    <tableColumn id="4" name="Conta Nível 1" dataDxfId="5"/>
+    <tableColumn id="5" name="Conta Nível 2" dataDxfId="4"/>
     <tableColumn id="6" name="Histórico" dataDxfId="1"/>
     <tableColumn id="7" name="Valor" dataDxfId="0"/>
   </tableColumns>
@@ -5558,7 +5683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6281,7 +6406,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7180,18 +7305,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="6" width="30.7109375" customWidth="1"/>
+    <col min="2" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="6" width="31.7109375" customWidth="1"/>
     <col min="7" max="7" width="45.42578125" customWidth="1"/>
     <col min="8" max="8" width="18.140625" customWidth="1"/>
     <col min="9" max="14" width="7.7109375" customWidth="1"/>
@@ -7352,7 +7475,7 @@
     <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations disablePrompts="1" count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E9">
       <formula1>PcEntradasN1</formula1>
     </dataValidation>
@@ -7378,37 +7501,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="2" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+    <col min="6" max="6" width="40.140625" customWidth="1"/>
+    <col min="7" max="7" width="41.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="9" max="14" width="11.7109375" customWidth="1"/>
     <col min="15" max="15" width="9.140625" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -7416,31 +7538,143 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-    </row>
-    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="3" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:8" ht="33.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="26">
+        <v>43147</v>
+      </c>
+      <c r="C6" s="26">
+        <v>43147</v>
+      </c>
+      <c r="D6" s="26">
+        <v>43147</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="31">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="26">
+        <v>43531</v>
+      </c>
+      <c r="C7" s="26">
+        <v>43466</v>
+      </c>
+      <c r="D7" s="26">
+        <v>43496</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="31">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="26">
+        <v>43496</v>
+      </c>
+      <c r="C8" s="26">
+        <v>43466</v>
+      </c>
+      <c r="D8" s="26">
+        <v>43496</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="31">
+        <v>4615.2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="26">
+        <v>43496</v>
+      </c>
+      <c r="C9" s="26">
+        <v>43466</v>
+      </c>
+      <c r="D9" s="26">
+        <v>43496</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="31">
+        <v>15384</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E10">
+      <formula1>SaidasNivel1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>